<commit_message>
30s mtm saved to local pos and export
</commit_message>
<xml_diff>
--- a/backtest results/long strangle expiry/IMP_long_strangle_200_1010.xlsx
+++ b/backtest results/long strangle expiry/IMP_long_strangle_200_1010.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniket.bhadane/Desktop/General/AniketBhadane.github.io/backtest results/long strangle expiry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCABEBBA-A7BE-F147-B1E0-131229F82731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A9C9BA-9C7A-E842-B2C2-9113701AC583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output" sheetId="1" r:id="rId1"/>
     <sheet name="200 dist" sheetId="2" r:id="rId2"/>
     <sheet name="100 dist" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="debit spread 100B-200S" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">output!$A$1:$S$84</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="41">
   <si>
     <t>instru</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>100 pnl rev</t>
+  </si>
+  <si>
+    <t>Debit spread 100 buy - 200 sell</t>
   </si>
 </sst>
 </file>
@@ -1548,7 +1551,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>'debit spread 100B-200S'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1571,7 +1574,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$21</c:f>
+              <c:f>'debit spread 100B-200S'!$E$2:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -3905,7 +3908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
@@ -9556,7 +9559,7 @@
   <dimension ref="A1:V37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T24" sqref="T24:T37"/>
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11150,7 +11153,7 @@
   <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S23" sqref="S23:S36"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12682,8 +12685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A49FB6-22DA-6C42-8969-7116F398F30B}">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12733,6 +12736,9 @@
         <f>D2+E3</f>
         <v>218.20000000000002</v>
       </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
       <c r="T2">
         <v>-44.400000000000006</v>
       </c>

</xml_diff>